<commit_message>
# refatoração de codigo 1
</commit_message>
<xml_diff>
--- a/tabela_resultados.xlsx
+++ b/tabela_resultados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pluca\OneDrive\Documents\Lucas\Estudos\APA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pluca\OneDrive\Documents\Lucas\Estudos\APA\APA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F7DC87-B8D6-4068-A880-BD6E4ABA1D8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAC7DBF-6F9B-4DB1-AF16-FBF62A3B4FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{7295AB22-DF39-475C-96BC-D1036519A718}"/>
   </bookViews>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578D373D-5DD1-4EE3-917E-7CC6007F7339}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -693,7 +693,7 @@
         <v>509</v>
       </c>
       <c r="D3">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="E3" s="2">
         <f>((C3-B3)/B3)</f>
@@ -706,7 +706,7 @@
         <v>34</v>
       </c>
       <c r="H3" s="2">
-        <f>((F3-B3)/B3)</f>
+        <f t="shared" ref="H3:H34" si="0">((F3-B3)/B3)</f>
         <v>-6.0747663551401869E-2</v>
       </c>
     </row>
@@ -721,20 +721,20 @@
         <v>665</v>
       </c>
       <c r="D4">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E34" si="0">((C4-B4)/B4)</f>
+        <f t="shared" ref="E4:E34" si="1">((C4-B4)/B4)</f>
         <v>0.31422924901185773</v>
       </c>
       <c r="F4">
         <v>558</v>
       </c>
       <c r="G4">
-        <v>35</v>
+        <v>437</v>
       </c>
       <c r="H4" s="2">
-        <f>((F4-B4)/B4)</f>
+        <f t="shared" si="0"/>
         <v>0.10276679841897234</v>
       </c>
     </row>
@@ -749,20 +749,20 @@
         <v>702</v>
       </c>
       <c r="D5">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2558139534883721</v>
       </c>
       <c r="F5">
         <v>564</v>
       </c>
       <c r="G5">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="2">
-        <f>((F5-B5)/B5)</f>
+        <f t="shared" si="0"/>
         <v>8.9445438282647581E-3</v>
       </c>
     </row>
@@ -777,20 +777,20 @@
         <v>444</v>
       </c>
       <c r="D6">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.8235294117647065E-2</v>
       </c>
       <c r="F6">
         <v>444</v>
       </c>
       <c r="G6">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H6" s="2">
-        <f>((F6-B6)/B6)</f>
+        <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
     </row>
@@ -805,20 +805,20 @@
         <v>501</v>
       </c>
       <c r="D7">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.3694267515923567E-2</v>
       </c>
       <c r="F7">
         <v>415</v>
       </c>
       <c r="G7">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="H7" s="2">
-        <f>((F7-B7)/B7)</f>
+        <f t="shared" si="0"/>
         <v>-0.11889596602972399</v>
       </c>
     </row>
@@ -833,20 +833,20 @@
         <v>595</v>
       </c>
       <c r="D8">
-        <v>76</v>
+        <v>149</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3097345132743362E-2</v>
       </c>
       <c r="F8">
         <v>509</v>
       </c>
       <c r="G8">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H8" s="2">
-        <f>((F8-B8)/B8)</f>
+        <f t="shared" si="0"/>
         <v>-9.9115044247787609E-2</v>
       </c>
     </row>
@@ -861,20 +861,20 @@
         <v>737</v>
       </c>
       <c r="D9">
-        <v>302</v>
+        <v>210</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29525483304042177</v>
       </c>
       <c r="F9">
         <v>613</v>
       </c>
       <c r="G9">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H9" s="2">
-        <f>((F9-B9)/B9)</f>
+        <f t="shared" si="0"/>
         <v>7.7328646748681895E-2</v>
       </c>
     </row>
@@ -889,20 +889,20 @@
         <v>598</v>
       </c>
       <c r="D10">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.26963906581740976</v>
       </c>
       <c r="F10">
         <v>598</v>
       </c>
       <c r="G10">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="2">
-        <f>((F10-B10)/B10)</f>
+        <f t="shared" si="0"/>
         <v>0.26963906581740976</v>
       </c>
     </row>
@@ -917,20 +917,20 @@
         <v>572</v>
       </c>
       <c r="D11">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5.4545454545454543E-2</v>
       </c>
       <c r="F11">
         <v>524</v>
       </c>
       <c r="G11">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H11" s="2">
-        <f>((F11-B11)/B11)</f>
+        <f t="shared" si="0"/>
         <v>-0.13388429752066117</v>
       </c>
     </row>
@@ -945,20 +945,20 @@
         <v>744</v>
       </c>
       <c r="D12">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4.2471042471042469E-2</v>
       </c>
       <c r="F12">
         <v>696</v>
       </c>
       <c r="G12">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="H12" s="2">
-        <f>((F12-B12)/B12)</f>
+        <f t="shared" si="0"/>
         <v>-0.10424710424710425</v>
       </c>
     </row>
@@ -973,20 +973,20 @@
         <v>716</v>
       </c>
       <c r="D13">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-7.8507078507078512E-2</v>
       </c>
       <c r="F13">
         <v>650</v>
       </c>
       <c r="G13">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H13" s="2">
-        <f>((F13-B13)/B13)</f>
+        <f t="shared" si="0"/>
         <v>-0.16344916344916344</v>
       </c>
     </row>
@@ -1001,20 +1001,20 @@
         <v>729</v>
       </c>
       <c r="D14">
-        <v>468</v>
+        <v>83</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.20495867768595041</v>
       </c>
       <c r="F14">
         <v>698</v>
       </c>
       <c r="G14">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H14" s="2">
-        <f>((F14-B14)/B14)</f>
+        <f t="shared" si="0"/>
         <v>0.1537190082644628</v>
       </c>
     </row>
@@ -1029,20 +1029,20 @@
         <v>1445</v>
       </c>
       <c r="D15">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2230769230769232</v>
       </c>
       <c r="F15">
         <v>1331</v>
       </c>
       <c r="G15">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H15" s="2">
-        <f>((F15-B15)/B15)</f>
+        <f t="shared" si="0"/>
         <v>1.0476923076923077</v>
       </c>
     </row>
@@ -1057,20 +1057,20 @@
         <v>1999</v>
       </c>
       <c r="D16">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.142550911039657</v>
       </c>
       <c r="F16">
         <v>1885</v>
       </c>
       <c r="G16">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H16" s="2">
-        <f>((F16-B16)/B16)</f>
+        <f t="shared" si="0"/>
         <v>1.0203644158628082</v>
       </c>
     </row>
@@ -1085,20 +1085,20 @@
         <v>2538</v>
       </c>
       <c r="D17">
-        <v>265</v>
+        <v>405</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7028753993610224</v>
       </c>
       <c r="F17">
         <v>2297</v>
       </c>
       <c r="G17">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="H17" s="2">
-        <f>((F17-B17)/B17)</f>
+        <f t="shared" si="0"/>
         <v>1.4462193823216187</v>
       </c>
     </row>
@@ -1113,20 +1113,20 @@
         <v>1335</v>
       </c>
       <c r="D18">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0350609756097562</v>
       </c>
       <c r="F18">
         <v>1300</v>
       </c>
       <c r="G18">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H18" s="2">
-        <f>((F18-B18)/B18)</f>
+        <f t="shared" si="0"/>
         <v>0.98170731707317072</v>
       </c>
     </row>
@@ -1141,20 +1141,20 @@
         <v>2049</v>
       </c>
       <c r="D19">
-        <v>262</v>
+        <v>413</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5580524344569289</v>
       </c>
       <c r="F19">
         <v>1914</v>
       </c>
       <c r="G19">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H19" s="2">
-        <f>((F19-B19)/B19)</f>
+        <f t="shared" si="0"/>
         <v>1.3895131086142323</v>
       </c>
     </row>
@@ -1169,20 +1169,20 @@
         <v>3255</v>
       </c>
       <c r="D20">
-        <v>320</v>
+        <v>437</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7057356608478802</v>
       </c>
       <c r="F20">
         <v>3120</v>
       </c>
       <c r="G20">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H20" s="2">
-        <f>((F20-B20)/B20)</f>
+        <f t="shared" si="0"/>
         <v>1.5935162094763091</v>
       </c>
     </row>
@@ -1197,20 +1197,20 @@
         <v>3773</v>
       </c>
       <c r="D21">
-        <v>303</v>
+        <v>362</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1233443708609272</v>
       </c>
       <c r="F21">
         <v>3563</v>
       </c>
       <c r="G21">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H21" s="2">
-        <f>((F21-B21)/B21)</f>
+        <f t="shared" si="0"/>
         <v>1.9495033112582782</v>
       </c>
     </row>
@@ -1225,20 +1225,20 @@
         <v>1680</v>
       </c>
       <c r="D22">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0947630922693268</v>
       </c>
       <c r="F22">
         <v>1645</v>
       </c>
       <c r="G22">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="H22" s="2">
-        <f>((F22-B22)/B22)</f>
+        <f t="shared" si="0"/>
         <v>1.0511221945137157</v>
       </c>
     </row>
@@ -1253,20 +1253,20 @@
         <v>2880</v>
       </c>
       <c r="D23">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0835117773019274</v>
       </c>
       <c r="F23">
         <v>2735</v>
       </c>
       <c r="G23">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H23" s="2">
-        <f>((F23-B23)/B23)</f>
+        <f t="shared" si="0"/>
         <v>1.9282655246252676</v>
       </c>
     </row>
@@ -1281,20 +1281,20 @@
         <v>4563</v>
       </c>
       <c r="D24">
-        <v>326</v>
+        <v>425</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0359281437125749</v>
       </c>
       <c r="F24">
         <v>4418</v>
       </c>
       <c r="G24">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H24" s="2">
-        <f>((F24-B24)/B24)</f>
+        <f t="shared" si="0"/>
         <v>1.9394544244843646</v>
       </c>
     </row>
@@ -1309,20 +1309,20 @@
         <v>6238</v>
       </c>
       <c r="D25">
-        <v>600</v>
+        <v>506</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1311258278145697</v>
       </c>
       <c r="F25">
         <v>5979</v>
       </c>
       <c r="G25">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H25" s="2">
-        <f>((F25-B25)/B25)</f>
+        <f t="shared" si="0"/>
         <v>2.9596026490066225</v>
       </c>
     </row>
@@ -1337,20 +1337,20 @@
         <v>2482</v>
       </c>
       <c r="D26">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6630901287553648</v>
       </c>
       <c r="F26">
         <v>2456</v>
       </c>
       <c r="G26">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H26" s="2">
-        <f>((F26-B26)/B26)</f>
+        <f t="shared" si="0"/>
         <v>1.6351931330472103</v>
       </c>
     </row>
@@ -1365,20 +1365,20 @@
         <v>5040</v>
       </c>
       <c r="D27">
-        <v>685</v>
+        <v>840</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8979591836734695</v>
       </c>
       <c r="F27">
         <v>4892</v>
       </c>
       <c r="G27">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="H27" s="2">
-        <f>((F27-B27)/B27)</f>
+        <f t="shared" si="0"/>
         <v>3.7541302235179788</v>
       </c>
     </row>
@@ -1393,20 +1393,20 @@
         <v>8049</v>
       </c>
       <c r="D28">
-        <v>684</v>
+        <v>466</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.922514619883041</v>
       </c>
       <c r="F28">
         <v>7901</v>
       </c>
       <c r="G28">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H28" s="2">
-        <f>((F28-B28)/B28)</f>
+        <f t="shared" si="0"/>
         <v>2.8503898635477585</v>
       </c>
     </row>
@@ -1421,20 +1421,20 @@
         <v>10591</v>
       </c>
       <c r="D29">
-        <v>941</v>
+        <v>2404</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1916666666666664</v>
       </c>
       <c r="F29">
         <v>10277</v>
       </c>
       <c r="G29">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="H29" s="2">
-        <f>((F29-B29)/B29)</f>
+        <f t="shared" si="0"/>
         <v>4.037745098039216</v>
       </c>
     </row>
@@ -1449,20 +1449,20 @@
         <v>4112</v>
       </c>
       <c r="D30">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.931166347992352</v>
       </c>
       <c r="F30">
         <v>4090</v>
       </c>
       <c r="G30">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H30" s="2">
-        <f>((F30-B30)/B30)</f>
+        <f t="shared" si="0"/>
         <v>2.910133843212237</v>
       </c>
     </row>
@@ -1477,20 +1477,20 @@
         <v>8180</v>
       </c>
       <c r="D31">
-        <v>1287</v>
+        <v>2101</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8923444976076556</v>
       </c>
       <c r="F31">
         <v>8002</v>
       </c>
       <c r="G31">
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="H31" s="2">
-        <f>((F31-B31)/B31)</f>
+        <f t="shared" si="0"/>
         <v>3.785885167464115</v>
       </c>
     </row>
@@ -1505,20 +1505,20 @@
         <v>17954</v>
       </c>
       <c r="D32">
-        <v>1089</v>
+        <v>1583</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4373107207752875</v>
       </c>
       <c r="F32">
         <v>17776</v>
       </c>
       <c r="G32">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="H32" s="2">
-        <f>((F32-B32)/B32)</f>
+        <f t="shared" si="0"/>
         <v>4.3834039975772257</v>
       </c>
     </row>
@@ -1533,20 +1533,20 @@
         <v>27567</v>
       </c>
       <c r="D33">
-        <v>1977</v>
+        <v>2054</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.3511057255377157</v>
       </c>
       <c r="F33">
         <v>27287</v>
       </c>
       <c r="G33">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="H33" s="2">
-        <f>((F33-B33)/B33)</f>
+        <f t="shared" si="0"/>
         <v>7.2662829445622537</v>
       </c>
     </row>
@@ -1561,20 +1561,20 @@
         <v>5254</v>
       </c>
       <c r="D34">
-        <v>461</v>
+        <v>365</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1423444976076556</v>
       </c>
       <c r="F34">
         <v>5217</v>
       </c>
       <c r="G34">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="H34" s="2">
-        <f>((F34-B34)/B34)</f>
+        <f t="shared" si="0"/>
         <v>2.1202153110047846</v>
       </c>
     </row>

</xml_diff>